<commit_message>
update Human Interface Guidelines
</commit_message>
<xml_diff>
--- a/iOS.xlsx
+++ b/iOS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="iOS 15 release notes" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>TabularData — это новая среда Swift, которую можно использовать для анализа табличных данных и управления ими. Можно использовать DataFrame для чтения файлов CSV и JSON, а также для объединения, группировки и агрегирования данных.</t>
   </si>
@@ -203,18 +203,9 @@
     <t xml:space="preserve">Picker: ввод различных значений (например выбор даты)  происходит с помощью барабана. </t>
   </si>
   <si>
-    <t>Иконка трех точек лежит горизонтально</t>
-  </si>
-  <si>
     <t>Стрелка «Назад» подписывается предыдущим экраном. Если на предыдущем экране заголовок был стандартным, то заголовок переходит из заголовка влево к стрелке. Если заголовок был широким, то заголовок поднимается вверх. Если название предыдущей страницы слишком длинное, оно заменяется на слово back.</t>
   </si>
   <si>
-    <t>Галочки используются как для radiobutton, так и для Checkbox.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Refresh Content Control вызывается жестом swipe down и «толкает» остальной контент вниз, при скроле контента исчезает.</t>
-  </si>
-  <si>
     <t>Стандартный control Steppers используется для ввода небольших значений.</t>
   </si>
   <si>
@@ -267,6 +258,18 @@
   </si>
   <si>
     <t>Human Interface Guidelines</t>
+  </si>
+  <si>
+    <t>Status Bar сообщает о времени, уровне заряда, качестве мобильной связи и Wi-Fi.</t>
+  </si>
+  <si>
+    <t>Refresh Content Control вызывается жестом swipe down и «толкает» остальной контент вниз, при скроле контента исчезает.</t>
+  </si>
+  <si>
+    <t>Control: галочки используются как для radiobutton, так и для Checkbox.</t>
+  </si>
+  <si>
+    <t>Иконка дополнительного меню (три точки) расположена горизонтально</t>
   </si>
 </sst>
 </file>
@@ -404,9 +407,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -421,17 +421,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,10 +730,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -754,7 +757,7 @@
     </row>
     <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <f>A4+1</f>
+        <f t="shared" ref="A5:A17" si="0">A4+1</f>
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -763,7 +766,7 @@
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -772,7 +775,7 @@
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -782,7 +785,7 @@
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -791,7 +794,7 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -800,7 +803,7 @@
     </row>
     <row r="10" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -809,7 +812,7 @@
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -818,7 +821,7 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -827,7 +830,7 @@
     </row>
     <row r="13" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -836,7 +839,7 @@
     </row>
     <row r="14" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -845,7 +848,7 @@
     </row>
     <row r="15" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -854,7 +857,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -863,7 +866,7 @@
     </row>
     <row r="17" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -881,315 +884,324 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="82.140625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="82.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <f t="shared" ref="A4:A35" si="0">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="18"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="16"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>1</v>
-      </c>
-      <c r="B3" s="13" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
-        <f>A3+1</f>
-        <v>2</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
-        <f>A4+1</f>
-        <v>3</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <f>A5+1</f>
-        <v>4</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <f>A6+1</f>
-        <v>5</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <f>A7+1</f>
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <f>A8+1</f>
-        <v>7</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <f>A9+1</f>
-        <v>8</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <f>A10+1</f>
-        <v>9</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
-        <f>A11+1</f>
-        <v>10</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <f>A12+1</f>
-        <v>11</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <f>A13+1</f>
-        <v>12</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <f>A14+1</f>
-        <v>13</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <f>A15+1</f>
-        <v>14</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
-        <f>A16+1</f>
-        <v>15</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <f>A17+1</f>
-        <v>16</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <f>A18+1</f>
-        <v>17</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <f>A19+1</f>
-        <v>18</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <f>A20+1</f>
-        <v>19</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <f>A21+1</f>
-        <v>20</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <f>A22+1</f>
-        <v>21</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <f>A23+1</f>
-        <v>22</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <f>A24+1</f>
-        <v>23</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
-        <f>A25+1</f>
-        <v>24</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
-        <f>A26+1</f>
-        <v>25</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
-        <f>A27+1</f>
-        <v>26</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
-        <f>A28+1</f>
-        <v>27</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
-        <f>A29+1</f>
-        <v>28</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
-        <f>A30+1</f>
-        <v>29</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
-        <f>A31+1</f>
-        <v>30</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
-        <f>A32+1</f>
-        <v>31</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
-        <f>A33+1</f>
-        <v>32</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1205,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1216,10 +1228,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -1243,7 +1255,7 @@
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <f>A4+1</f>
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1252,7 +1264,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1261,7 +1273,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1270,7 +1282,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1279,7 +1291,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1288,7 +1300,7 @@
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1297,7 +1309,7 @@
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1306,7 +1318,7 @@
     </row>
     <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1315,7 +1327,7 @@
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1324,7 +1336,7 @@
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1333,7 +1345,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1342,7 +1354,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1351,7 +1363,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1360,7 +1372,7 @@
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1369,7 +1381,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1378,7 +1390,7 @@
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1387,7 +1399,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1396,7 +1408,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1405,7 +1417,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1414,7 +1426,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1423,7 +1435,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <f>A24+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1432,7 +1444,7 @@
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1441,7 +1453,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <f>A26+1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1450,7 +1462,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <f>A27+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -1459,7 +1471,7 @@
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <f>A28+1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1468,7 +1480,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1477,7 +1489,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <f>A30+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1486,7 +1498,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1495,7 +1507,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <f>A32+1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B33" s="4" t="s">

</xml_diff>